<commit_message>
C9 up to 9.3 department Specific budget allocation tables are added in both excel and word file
</commit_message>
<xml_diff>
--- a/Criterion 9/C9 Tables.xlsx
+++ b/Criterion 9/C9 Tables.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Heading Chapter" sheetId="1" r:id="rId1"/>
     <sheet name="9.1.1 availibilty of vision and" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="9.2 Income at institute " sheetId="3" r:id="rId3"/>
+    <sheet name="9.3 Department Specific budget" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>CRITERION 9</t>
   </si>
@@ -88,13 +89,946 @@
   </si>
   <si>
     <t>Notice boards</t>
+  </si>
+  <si>
+    <t>Fee</t>
+  </si>
+  <si>
+    <t>Govt.</t>
+  </si>
+  <si>
+    <t>Grant(s)</t>
+  </si>
+  <si>
+    <t>Non-recurring</t>
+  </si>
+  <si>
+    <r>
+      <t>Total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>No.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>students</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sources</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Recurring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>including</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Salaries</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Special Projects/Any</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>other,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>specify</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Expenses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>per</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>student</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Income</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm1: 2019-20</t>
+    </r>
+  </si>
+  <si>
+    <t>For CFYm1 : 2019-20</t>
+  </si>
+  <si>
+    <r>
+      <t>Actual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>expenses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm1 (till March 31St)</t>
+    </r>
+  </si>
+  <si>
+    <t>For CFYm2 : 2018-19</t>
+  </si>
+  <si>
+    <r>
+      <t>Total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Income</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm2: 2018-19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>No.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>students</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Actual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>expenses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm2 (till March 31St)</t>
+    </r>
+  </si>
+  <si>
+    <t>For CFYm2 : 2017-18</t>
+  </si>
+  <si>
+    <r>
+      <t>Total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Income</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm3: 2017-18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Actual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>expenses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm3 (till March 31St)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>No.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>students</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>CFYm3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>Recurring</t>
+  </si>
+  <si>
+    <t>Non-Recurring</t>
+  </si>
+  <si>
+    <t>Total Budget in CFY:</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Actual expenses in CFY (till 31st March ):</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFYm1 : </t>
+  </si>
+  <si>
+    <t>Total Budget in CFYm1:</t>
+  </si>
+  <si>
+    <t>Actual expenses in CFYm1 (till 31st March ):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFYm2 : </t>
+  </si>
+  <si>
+    <t>Total Budget in CFYm2:</t>
+  </si>
+  <si>
+    <t>Actual expenses in CFYm2 (till 31st March ):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFYm3 : </t>
+  </si>
+  <si>
+    <t>Total Budget in CFYm3:</t>
+  </si>
+  <si>
+    <t>Actual expenses in CFYm3 (till 31st March ):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFY :  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +1061,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,6 +1143,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,12 +1723,568 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="F2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="2:9" s="7" customFormat="1" ht="45" customHeight="1">
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="38.25">
+      <c r="B4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="60" customHeight="1">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="F8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="2:9" ht="38.25">
+      <c r="B9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="38.25">
+      <c r="B10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="42.75" customHeight="1">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="F14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="2:9" ht="38.25">
+      <c r="B15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="38.25">
+      <c r="B16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="38.25" customHeight="1">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="D2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="2:6" s="2" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" s="2" customFormat="1" ht="12.75">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="D12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:6" ht="25.5" customHeight="1">
+      <c r="B13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="D22" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="8"/>
+      <c r="C24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="D32" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="8"/>
+      <c r="C34" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+    </row>
+  </sheetData>
+  <sortState ref="B35:B39">
+    <sortCondition ref="B35"/>
+  </sortState>
+  <mergeCells count="16">
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
C9 Information Realted to Coomunity delopment added
</commit_message>
<xml_diff>
--- a/Criterion 9/C9 Tables.xlsx
+++ b/Criterion 9/C9 Tables.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Heading Chapter" sheetId="1" r:id="rId1"/>
     <sheet name="9.1.1 availibilty of vision and" sheetId="2" r:id="rId2"/>
     <sheet name="9.2 Income at institute " sheetId="3" r:id="rId3"/>
     <sheet name="9.3 Department Specific budget" sheetId="4" r:id="rId4"/>
+    <sheet name="9.5 Community Development" sheetId="5" r:id="rId5"/>
+    <sheet name="9.6 Alumini Performance and con" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -1149,14 +1151,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1166,6 +1162,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1498,7 +1500,7 @@
   <dimension ref="B4:E29"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D25"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1726,7 +1728,7 @@
   <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I17"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1740,190 +1742,190 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="2:9" s="7" customFormat="1" ht="45" customHeight="1">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="38.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="60" customHeight="1">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:9" ht="38.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9" t="s">
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="38.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="42.75" customHeight="1">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:9" ht="38.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="9" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="38.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="38.25" customHeight="1">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1934,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1954,77 +1956,77 @@
       <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:6" s="2" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="2:6" s="2" customFormat="1" ht="12.75">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="12" spans="2:6">
       <c r="D12" s="15" t="s">
@@ -2033,77 +2035,77 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:6" ht="25.5" customHeight="1">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="22" spans="2:6">
       <c r="D22" s="15" t="s">
@@ -2112,77 +2114,77 @@
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="14"/>
+      <c r="E23" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="8"/>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="32" spans="2:6">
       <c r="D32" s="15" t="s">
@@ -2191,88 +2193,83 @@
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8" t="s">
+      <c r="D33" s="14"/>
+      <c r="E33" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="8"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="8"/>
-      <c r="C34" s="9" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="2:6">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="2:6">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="2:6">
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39" spans="2:6">
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
     </row>
   </sheetData>
   <sortState ref="B35:B39">
     <sortCondition ref="B35"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="D32:E32"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="E33:F33"/>
@@ -2284,7 +2281,36 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
C9 9.5 Community Development Tables and Data added 2016-17-2018
</commit_message>
<xml_diff>
--- a/Criterion 9/C9 Tables.xlsx
+++ b/Criterion 9/C9 Tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="135">
   <si>
     <t>CRITERION 9</t>
   </si>
@@ -1024,13 +1024,226 @@
   </si>
   <si>
     <t xml:space="preserve">CFY :  </t>
+  </si>
+  <si>
+    <t>Sr.No</t>
+  </si>
+  <si>
+    <t>Name of Training program  conducted</t>
+  </si>
+  <si>
+    <t>Duration of Training</t>
+  </si>
+  <si>
+    <t>(In Weeks)</t>
+  </si>
+  <si>
+    <t>Place Of Training Conducted</t>
+  </si>
+  <si>
+    <t>Number of Participants</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Organizer</t>
+  </si>
+  <si>
+    <t>Name of Trainer</t>
+  </si>
+  <si>
+    <t>GovtResi Women’s polytechnic latur</t>
+  </si>
+  <si>
+    <t>Aanandwadi Ta. SururAnantpal Dist. Latur</t>
+  </si>
+  <si>
+    <t>Smt. JayshreeManshingKasbe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Computer </t>
+  </si>
+  <si>
+    <t>Rapka</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Duration of Training (In Weeks)</t>
+  </si>
+  <si>
+    <t>Training Organizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fashion Designing  </t>
+  </si>
+  <si>
+    <t>Smt. Jayshree Manshing Kasbe</t>
+  </si>
+  <si>
+    <t>Inamwadi Ta Nilanga Dist Latur</t>
+  </si>
+  <si>
+    <t>Aanandwadi Ta Shirur  Anantpal Dist. Latur</t>
+  </si>
+  <si>
+    <t>Government Residential Womens Polytechnic Latur</t>
+  </si>
+  <si>
+    <t>Smt. Priyanka Suresh Gobade</t>
+  </si>
+  <si>
+    <t>Details of Training Conducted During Year 2016-17</t>
+  </si>
+  <si>
+    <t>Details of Training Conducted During Year 2017-18</t>
+  </si>
+  <si>
+    <t>Basic Computer</t>
+  </si>
+  <si>
+    <t>Fashion Dinging (Handwork)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTP Computer </t>
+  </si>
+  <si>
+    <t>Panchincoli</t>
+  </si>
+  <si>
+    <t>Ta.NilangaDistLatur</t>
+  </si>
+  <si>
+    <t>Mr.GaneshBhosle</t>
+  </si>
+  <si>
+    <t>Dapka (TANDA) Dist Latur</t>
+  </si>
+  <si>
+    <t>Smt. Mukta Bibishan Bansode</t>
+  </si>
+  <si>
+    <t>Beauty parlour and hairdressing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garment Designing </t>
+  </si>
+  <si>
+    <t>Shirur Anantpal Dist. Latur</t>
+  </si>
+  <si>
+    <t>Aanandwadi Ta. Shirur Anantpal Dist. Latur</t>
+  </si>
+  <si>
+    <t>Panchincholi Ta. Nilanga Dist Latur</t>
+  </si>
+  <si>
+    <t>Smt. B.P. Shendre</t>
+  </si>
+  <si>
+    <t>Smt. Chaya Tulshiram Gargatte</t>
+  </si>
+  <si>
+    <t>Smt. Jayshree Manshing Kasabe</t>
+  </si>
+  <si>
+    <t>Mr. Ganesh Bhosle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware </t>
+  </si>
+  <si>
+    <t>Beautician &amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heir dressing    </t>
+  </si>
+  <si>
+    <t>Arvi Dist. Latur</t>
+  </si>
+  <si>
+    <t>Smt. VasudhaAdsule</t>
+  </si>
+  <si>
+    <t>Baratkam  (Handwork)</t>
+  </si>
+  <si>
+    <t>BanegoanTa.AusaDist.Latur</t>
+  </si>
+  <si>
+    <t>Smt. Tor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fashion Dinging </t>
+  </si>
+  <si>
+    <t>Beauty Parlier</t>
+  </si>
+  <si>
+    <t>Shindijawalga Ta Ausa</t>
+  </si>
+  <si>
+    <t>Dist. Latur</t>
+  </si>
+  <si>
+    <t>Smt. Malan DilipGholap</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beauty Parlier </t>
+  </si>
+  <si>
+    <t>KeshavnagarDistLatur</t>
+  </si>
+  <si>
+    <t>Mr.vandnasugrivGaikwad</t>
+  </si>
+  <si>
+    <t>Advance Corse In Fashion Technology</t>
+  </si>
+  <si>
+    <t>Micron Work</t>
+  </si>
+  <si>
+    <t>Arvi Ta LaturDistLatur</t>
+  </si>
+  <si>
+    <t>Smt.VasudhaAdsule</t>
+  </si>
+  <si>
+    <t>Haribhau Nagar Latur</t>
+  </si>
+  <si>
+    <t>Smt.JyotiMarkade</t>
+  </si>
+  <si>
+    <t>Himayat Nagar Latur</t>
+  </si>
+  <si>
+    <t>Smt.AyeshaPathan</t>
+  </si>
+  <si>
+    <t>Gandhi Nagar Latur</t>
+  </si>
+  <si>
+    <t>Smt.ArunaDiggikar</t>
+  </si>
+  <si>
+    <t>Prakash  Nagar Latur</t>
+  </si>
+  <si>
+    <t>Smt. Mina Kulkarni</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1091,6 +1304,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1100,7 +1333,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1123,11 +1356,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1163,14 +1490,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1742,23 +2123,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:9" s="7" customFormat="1" ht="45" customHeight="1">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
       <c r="I3" s="8" t="s">
         <v>28</v>
       </c>
@@ -1800,23 +2181,23 @@
       <c r="I5" s="9"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="2:9" ht="38.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
@@ -1858,23 +2239,23 @@
       <c r="I11" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="2:9" ht="38.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
@@ -1956,20 +2337,20 @@
       <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:6" s="2" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="2:6" s="2" customFormat="1" ht="12.75">
-      <c r="B4" s="14"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
@@ -2035,20 +2416,20 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:6" ht="25.5" customHeight="1">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="14"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
@@ -2114,20 +2495,20 @@
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14" t="s">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
@@ -2193,20 +2574,20 @@
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14" t="s">
+      <c r="D33" s="13"/>
+      <c r="E33" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="14"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="14"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="8" t="s">
         <v>27</v>
       </c>
@@ -2293,24 +2674,945 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A23:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="23" spans="1:8" ht="23.25" customHeight="1">
+      <c r="A23" s="32"/>
+      <c r="B23" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" customHeight="1">
+      <c r="B24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4">
+        <v>4</v>
+      </c>
+      <c r="F25" s="4">
+        <v>5</v>
+      </c>
+      <c r="G25" s="4">
+        <v>6</v>
+      </c>
+      <c r="H25" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="36" customHeight="1">
+      <c r="B26" s="31">
+        <v>1</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="11">
+        <v>12</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="11">
+        <v>20</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="53.25" customHeight="1">
+      <c r="B27" s="31">
+        <v>2</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="11">
+        <v>12</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="11">
+        <v>20</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="48.75" customHeight="1">
+      <c r="B28" s="31">
+        <v>3</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="11">
+        <v>12</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="11">
+        <v>25</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="53.25" customHeight="1">
+      <c r="B29" s="31">
+        <v>4</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="11">
+        <v>12</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="11">
+        <v>20</v>
+      </c>
+      <c r="G29" s="30"/>
+      <c r="H29" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="35.25" customHeight="1">
+      <c r="B30" s="31">
+        <v>5</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="11">
+        <v>12</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="11">
+        <v>21</v>
+      </c>
+      <c r="G30" s="30"/>
+      <c r="H30" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="25.5" customHeight="1">
+      <c r="B31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="11">
+        <v>5</v>
+      </c>
+      <c r="D31" s="11">
+        <v>60</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11">
+        <v>106</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+    </row>
+    <row r="33" spans="2:8" ht="20.25">
+      <c r="E33" s="22"/>
+    </row>
+    <row r="34" spans="2:8" ht="24" customHeight="1">
+      <c r="B34" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+    </row>
+    <row r="35" spans="2:8" ht="65.25" customHeight="1">
+      <c r="B35" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="18" customHeight="1">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2</v>
+      </c>
+      <c r="D36" s="4">
+        <v>3</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4</v>
+      </c>
+      <c r="F36" s="4">
+        <v>5</v>
+      </c>
+      <c r="G36" s="4">
+        <v>6</v>
+      </c>
+      <c r="H36" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="36" customHeight="1">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="23">
+        <v>12</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="23">
+        <v>20</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="53.25" customHeight="1">
+      <c r="B38" s="4">
+        <v>2</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="11">
+        <v>12</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="11">
+        <v>21</v>
+      </c>
+      <c r="G38" s="25"/>
+      <c r="H38" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="26.25" customHeight="1">
+      <c r="B39" s="4">
+        <v>3</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="11">
+        <v>12</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="11">
+        <v>18</v>
+      </c>
+      <c r="G39" s="26"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="2:8" ht="29.25" customHeight="1">
+      <c r="B40" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="11">
+        <v>3</v>
+      </c>
+      <c r="D40" s="11">
+        <v>36</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11">
+        <v>59</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="B34:H34"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1"/>
+    <row r="4" spans="2:8" ht="89.25" customHeight="1">
+      <c r="B4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="54.75" thickBot="1">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="2:8" ht="18.75" thickBot="1">
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17">
+        <v>2</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17">
+        <v>4</v>
+      </c>
+      <c r="F6" s="17">
+        <v>5</v>
+      </c>
+      <c r="G6" s="17">
+        <v>6</v>
+      </c>
+      <c r="H6" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="54">
+      <c r="B7" s="20">
+        <v>1</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="20">
+        <v>12</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="20">
+        <v>13</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="72.75" thickBot="1">
+      <c r="B8" s="21"/>
+      <c r="C8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="2:8" ht="71.25" customHeight="1">
+      <c r="B9" s="20">
+        <v>2</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="20">
+        <v>12</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="20">
+        <v>21</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="54.75" thickBot="1">
+      <c r="B10" s="21"/>
+      <c r="C10" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="2:8" ht="126.75" thickBot="1">
+      <c r="B11" s="18">
+        <v>3</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="17">
+        <v>12</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="17">
+        <v>19</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="144.75" thickBot="1">
+      <c r="B12" s="18">
+        <v>4</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="17">
+        <v>12</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="17">
+        <v>22</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="144.75" thickBot="1">
+      <c r="B13" s="18">
+        <v>5</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="17">
+        <v>12</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="17">
+        <v>20</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="53.25" customHeight="1">
+      <c r="B14" s="20">
+        <v>6</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="20">
+        <v>12</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="20">
+        <v>18</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="72.75" thickBot="1">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="2:8" ht="110.25" customHeight="1">
+      <c r="B16" s="20">
+        <v>7</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="20">
+        <v>12</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="20">
+        <v>21</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="2:8" ht="89.25" customHeight="1">
+      <c r="B18" s="20">
+        <v>8</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="20">
+        <v>12</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="20">
+        <v>21</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="36.75" thickBot="1">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="2:8" ht="126.75" thickBot="1">
+      <c r="B20" s="18">
+        <v>9</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="17">
+        <v>12</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="17">
+        <v>16</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="144.75" thickBot="1">
+      <c r="B21" s="18">
+        <v>10</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="17">
+        <v>12</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="17">
+        <v>22</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="144.75" thickBot="1">
+      <c r="B22" s="18">
+        <v>11</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="17">
+        <v>4</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="17">
+        <v>15</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="126.75" thickBot="1">
+      <c r="B23" s="18">
+        <v>12</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="17">
+        <v>4</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" s="17">
+        <v>13</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="126.75" thickBot="1">
+      <c r="B24" s="18">
+        <v>13</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="17">
+        <v>12</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="17">
+        <v>21</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="126.75" thickBot="1">
+      <c r="B25" s="18">
+        <v>14</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="17">
+        <v>12</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="17">
+        <v>20</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="71.25" customHeight="1">
+      <c r="B26" s="20">
+        <v>15</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="20">
+        <v>12</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="20">
+        <v>20</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="54.75" thickBot="1">
+      <c r="B27" s="21"/>
+      <c r="C27" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="2:8" ht="126.75" thickBot="1">
+      <c r="B28" s="18">
+        <v>16</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="17">
+        <v>12</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="17">
+        <v>20</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="144.75" thickBot="1">
+      <c r="B29" s="18">
+        <v>17</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="17">
+        <v>12</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="17">
+        <v>21</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="18.75" thickBot="1">
+      <c r="B30" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="17">
+        <v>17</v>
+      </c>
+      <c r="D30" s="17">
+        <v>188</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17">
+        <v>323</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="41">
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
C9 Community development Traning added 2016-17
</commit_message>
<xml_diff>
--- a/Criterion 9/C9 Tables.xlsx
+++ b/Criterion 9/C9 Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Heading Chapter" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>CRITERION 9</t>
   </si>
@@ -1032,36 +1032,15 @@
     <t>Name of Training program  conducted</t>
   </si>
   <si>
-    <t>Duration of Training</t>
-  </si>
-  <si>
-    <t>(In Weeks)</t>
-  </si>
-  <si>
     <t>Place Of Training Conducted</t>
   </si>
   <si>
     <t>Number of Participants</t>
   </si>
   <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Organizer</t>
-  </si>
-  <si>
     <t>Name of Trainer</t>
   </si>
   <si>
-    <t>GovtResi Women’s polytechnic latur</t>
-  </si>
-  <si>
-    <t>Aanandwadi Ta. SururAnantpal Dist. Latur</t>
-  </si>
-  <si>
-    <t>Smt. JayshreeManshingKasbe</t>
-  </si>
-  <si>
     <t xml:space="preserve">Basic Computer </t>
   </si>
   <si>
@@ -1110,15 +1089,6 @@
     <t xml:space="preserve">DTP Computer </t>
   </si>
   <si>
-    <t>Panchincoli</t>
-  </si>
-  <si>
-    <t>Ta.NilangaDistLatur</t>
-  </si>
-  <si>
-    <t>Mr.GaneshBhosle</t>
-  </si>
-  <si>
     <t>Dapka (TANDA) Dist Latur</t>
   </si>
   <si>
@@ -1150,100 +1120,13 @@
   </si>
   <si>
     <t>Mr. Ganesh Bhosle</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Computer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardware </t>
-  </si>
-  <si>
-    <t>Beautician &amp;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heir dressing    </t>
-  </si>
-  <si>
-    <t>Arvi Dist. Latur</t>
-  </si>
-  <si>
-    <t>Smt. VasudhaAdsule</t>
-  </si>
-  <si>
-    <t>Baratkam  (Handwork)</t>
-  </si>
-  <si>
-    <t>BanegoanTa.AusaDist.Latur</t>
-  </si>
-  <si>
-    <t>Smt. Tor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fashion Dinging </t>
-  </si>
-  <si>
-    <t>Beauty Parlier</t>
-  </si>
-  <si>
-    <t>Shindijawalga Ta Ausa</t>
-  </si>
-  <si>
-    <t>Dist. Latur</t>
-  </si>
-  <si>
-    <t>Smt. Malan DilipGholap</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Beauty Parlier </t>
-  </si>
-  <si>
-    <t>KeshavnagarDistLatur</t>
-  </si>
-  <si>
-    <t>Mr.vandnasugrivGaikwad</t>
-  </si>
-  <si>
-    <t>Advance Corse In Fashion Technology</t>
-  </si>
-  <si>
-    <t>Micron Work</t>
-  </si>
-  <si>
-    <t>Arvi Ta LaturDistLatur</t>
-  </si>
-  <si>
-    <t>Smt.VasudhaAdsule</t>
-  </si>
-  <si>
-    <t>Haribhau Nagar Latur</t>
-  </si>
-  <si>
-    <t>Smt.JyotiMarkade</t>
-  </si>
-  <si>
-    <t>Himayat Nagar Latur</t>
-  </si>
-  <si>
-    <t>Smt.AyeshaPathan</t>
-  </si>
-  <si>
-    <t>Gandhi Nagar Latur</t>
-  </si>
-  <si>
-    <t>Smt.ArunaDiggikar</t>
-  </si>
-  <si>
-    <t>Prakash  Nagar Latur</t>
-  </si>
-  <si>
-    <t>Smt. Mina Kulkarni</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1305,12 +1188,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -1333,7 +1210,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1354,63 +1231,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1454,7 +1274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1490,6 +1310,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1499,58 +1340,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2123,23 +1925,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="2:9" s="7" customFormat="1" ht="45" customHeight="1">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="8" t="s">
         <v>28</v>
       </c>
@@ -2181,23 +1983,23 @@
       <c r="I5" s="9"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="2:9" ht="38.25">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
@@ -2239,23 +2041,23 @@
       <c r="I11" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="2:9" ht="38.25">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
@@ -2331,26 +2133,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="15"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="2:6" s="2" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="2:6" s="2" customFormat="1" ht="12.75">
-      <c r="B4" s="13"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
@@ -2410,26 +2212,26 @@
       <c r="F9" s="10"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="2:6" ht="25.5" customHeight="1">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="13"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
@@ -2489,26 +2291,26 @@
       <c r="F19" s="10"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13" t="s">
+      <c r="D23" s="20"/>
+      <c r="E23" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="13"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
@@ -2568,26 +2370,26 @@
       <c r="F29" s="10"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13" t="s">
+      <c r="D33" s="20"/>
+      <c r="E33" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="13"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="13"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="8" t="s">
         <v>27</v>
       </c>
@@ -2676,8 +2478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A23:H40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2692,16 +2494,16 @@
   </cols>
   <sheetData>
     <row r="23" spans="1:8" ht="23.25" customHeight="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" ht="60" customHeight="1">
       <c r="B24" s="4" t="s">
@@ -2711,19 +2513,19 @@
         <v>65</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="19.5" customHeight="1">
@@ -2750,115 +2552,115 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="36" customHeight="1">
-      <c r="B26" s="31">
+      <c r="B26" s="17">
         <v>1</v>
       </c>
-      <c r="C26" s="31" t="s">
-        <v>89</v>
+      <c r="C26" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="11">
         <v>12</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F26" s="11">
         <v>20</v>
       </c>
-      <c r="G26" s="30" t="s">
-        <v>85</v>
+      <c r="G26" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="53.25" customHeight="1">
-      <c r="B27" s="31">
+      <c r="B27" s="17">
         <v>2</v>
       </c>
-      <c r="C27" s="31" t="s">
-        <v>97</v>
+      <c r="C27" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="D27" s="11">
         <v>12</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F27" s="11">
         <v>20</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="11" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="48.75" customHeight="1">
-      <c r="B28" s="31">
+      <c r="B28" s="17">
         <v>3</v>
       </c>
-      <c r="C28" s="31" t="s">
-        <v>98</v>
+      <c r="C28" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="D28" s="11">
         <v>12</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F28" s="11">
         <v>25</v>
       </c>
-      <c r="G28" s="30"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="11" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="53.25" customHeight="1">
-      <c r="B29" s="31">
+      <c r="B29" s="17">
         <v>4</v>
       </c>
-      <c r="C29" s="31" t="s">
-        <v>90</v>
+      <c r="C29" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="D29" s="11">
         <v>12</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F29" s="11">
         <v>20</v>
       </c>
-      <c r="G29" s="30"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="11" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="35.25" customHeight="1">
-      <c r="B30" s="31">
+      <c r="B30" s="17">
         <v>5</v>
       </c>
-      <c r="C30" s="31" t="s">
-        <v>91</v>
+      <c r="C30" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="D30" s="11">
         <v>12</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F30" s="11">
         <v>21</v>
       </c>
-      <c r="G30" s="30"/>
+      <c r="G30" s="24"/>
       <c r="H30" s="11" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="25.5" customHeight="1">
       <c r="B31" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C31" s="11">
         <v>5</v>
@@ -2874,40 +2676,40 @@
       <c r="H31" s="11"/>
     </row>
     <row r="33" spans="2:8" ht="20.25">
-      <c r="E33" s="22"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="2:8" ht="24" customHeight="1">
-      <c r="B34" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
+      <c r="B34" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="2:8" ht="65.25" customHeight="1">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="28" t="s">
+      <c r="D35" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="F35" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="H35" s="28" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="18" customHeight="1">
@@ -2937,68 +2739,68 @@
       <c r="B37" s="4">
         <v>1</v>
       </c>
-      <c r="C37" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="23">
+      <c r="C37" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="14">
         <v>12</v>
       </c>
-      <c r="E37" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="23">
+      <c r="E37" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="14">
         <v>20</v>
       </c>
-      <c r="G37" s="24" t="s">
-        <v>85</v>
+      <c r="G37" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="53.25" customHeight="1">
       <c r="B38" s="4">
         <v>2</v>
       </c>
-      <c r="C38" s="29" t="s">
-        <v>81</v>
+      <c r="C38" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="D38" s="11">
         <v>12</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F38" s="11">
         <v>21</v>
       </c>
-      <c r="G38" s="25"/>
+      <c r="G38" s="26"/>
       <c r="H38" s="11" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="26.25" customHeight="1">
       <c r="B39" s="4">
         <v>3</v>
       </c>
-      <c r="C39" s="31" t="s">
-        <v>76</v>
+      <c r="C39" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="D39" s="11">
         <v>12</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F39" s="11">
         <v>18</v>
       </c>
-      <c r="G39" s="26"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="11"/>
     </row>
     <row r="40" spans="2:8" ht="29.25" customHeight="1">
       <c r="B40" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C40" s="11">
         <v>3</v>
@@ -3027,592 +2829,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:H30"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="4" spans="2:8" ht="89.25" customHeight="1">
-      <c r="B4" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="54.75" thickBot="1">
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="21"/>
-    </row>
-    <row r="6" spans="2:8" ht="18.75" thickBot="1">
-      <c r="B6" s="18">
-        <v>1</v>
-      </c>
-      <c r="C6" s="17">
-        <v>2</v>
-      </c>
-      <c r="D6" s="17">
-        <v>3</v>
-      </c>
-      <c r="E6" s="17">
-        <v>4</v>
-      </c>
-      <c r="F6" s="17">
-        <v>5</v>
-      </c>
-      <c r="G6" s="17">
-        <v>6</v>
-      </c>
-      <c r="H6" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="54">
-      <c r="B7" s="20">
-        <v>1</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="20">
-        <v>12</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" s="20">
-        <v>13</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="72.75" thickBot="1">
-      <c r="B8" s="21"/>
-      <c r="C8" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="2:8" ht="71.25" customHeight="1">
-      <c r="B9" s="20">
-        <v>2</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="20">
-        <v>12</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" s="20">
-        <v>21</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="54.75" thickBot="1">
-      <c r="B10" s="21"/>
-      <c r="C10" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="2:8" ht="126.75" thickBot="1">
-      <c r="B11" s="18">
-        <v>3</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="17">
-        <v>12</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="F11" s="17">
-        <v>19</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="144.75" thickBot="1">
-      <c r="B12" s="18">
-        <v>4</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" s="17">
-        <v>12</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="17">
-        <v>22</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="144.75" thickBot="1">
-      <c r="B13" s="18">
-        <v>5</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="17">
-        <v>12</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="17">
-        <v>20</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="53.25" customHeight="1">
-      <c r="B14" s="20">
-        <v>6</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="20">
-        <v>12</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" s="20">
-        <v>18</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="72.75" thickBot="1">
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="2:8" ht="110.25" customHeight="1">
-      <c r="B16" s="20">
-        <v>7</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="20">
-        <v>12</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="20">
-        <v>21</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-    </row>
-    <row r="18" spans="2:8" ht="89.25" customHeight="1">
-      <c r="B18" s="20">
-        <v>8</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D18" s="20">
-        <v>12</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="20">
-        <v>21</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="36.75" thickBot="1">
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-    </row>
-    <row r="20" spans="2:8" ht="126.75" thickBot="1">
-      <c r="B20" s="18">
-        <v>9</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20" s="17">
-        <v>12</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="17">
-        <v>16</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="144.75" thickBot="1">
-      <c r="B21" s="18">
-        <v>10</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="17">
-        <v>12</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="17">
-        <v>22</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="144.75" thickBot="1">
-      <c r="B22" s="18">
-        <v>11</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="17">
-        <v>4</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="17">
-        <v>15</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="126.75" thickBot="1">
-      <c r="B23" s="18">
-        <v>12</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="17">
-        <v>4</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" s="17">
-        <v>13</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="126.75" thickBot="1">
-      <c r="B24" s="18">
-        <v>13</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="17">
-        <v>12</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" s="17">
-        <v>21</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="126.75" thickBot="1">
-      <c r="B25" s="18">
-        <v>14</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="17">
-        <v>12</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" s="17">
-        <v>20</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="71.25" customHeight="1">
-      <c r="B26" s="20">
-        <v>15</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="20">
-        <v>12</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" s="20">
-        <v>20</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="54.75" thickBot="1">
-      <c r="B27" s="21"/>
-      <c r="C27" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="2:8" ht="126.75" thickBot="1">
-      <c r="B28" s="18">
-        <v>16</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="17">
-        <v>12</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="F28" s="17">
-        <v>20</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="144.75" thickBot="1">
-      <c r="B29" s="18">
-        <v>17</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="17">
-        <v>12</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="17">
-        <v>21</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="18.75" thickBot="1">
-      <c r="B30" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="17">
-        <v>17</v>
-      </c>
-      <c r="D30" s="17">
-        <v>188</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
-        <v>323</v>
-      </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
C9 Community Development Training Program for 2018-19 added
</commit_message>
<xml_diff>
--- a/Criterion 9/C9 Tables.xlsx
+++ b/Criterion 9/C9 Tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="138">
   <si>
     <t>CRITERION 9</t>
   </si>
@@ -1041,6 +1041,9 @@
     <t>Name of Trainer</t>
   </si>
   <si>
+    <t>Aanandwadi Ta. SururAnantpal Dist. Latur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basic Computer </t>
   </si>
   <si>
@@ -1120,13 +1123,136 @@
   </si>
   <si>
     <t>Mr. Ganesh Bhosle</t>
+  </si>
+  <si>
+    <t>Arvi Dist. Latur</t>
+  </si>
+  <si>
+    <t>Baratkam  (Handwork)</t>
+  </si>
+  <si>
+    <t>Smt. Tor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fashion Dinging </t>
+  </si>
+  <si>
+    <t>Advance Corse In Fashion Technology</t>
+  </si>
+  <si>
+    <t>Micron Work</t>
+  </si>
+  <si>
+    <t>Haribhau Nagar Latur</t>
+  </si>
+  <si>
+    <t>Himayat Nagar Latur</t>
+  </si>
+  <si>
+    <t>Gandhi Nagar Latur</t>
+  </si>
+  <si>
+    <t>Details of Community Developement Training Conducted During Year 2018-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Computer Hardware</t>
+  </si>
+  <si>
+    <t>Panchincoli Tal Nilanga Dist Latur</t>
+  </si>
+  <si>
+    <t>Governement Residential Womens Polytechnic, Latur</t>
+  </si>
+  <si>
+    <t>Mr Ganesh Bhosle</t>
+  </si>
+  <si>
+    <t>Beautician and Hairdressing</t>
+  </si>
+  <si>
+    <t>Smt. Vasudha Adsule</t>
+  </si>
+  <si>
+    <t>BanegoanTa. Ausa Dist. Latur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fashion Designing </t>
+  </si>
+  <si>
+    <t>Beauty Parlour</t>
+  </si>
+  <si>
+    <t>Shindijawalga Ta Ausa Dist Latur</t>
+  </si>
+  <si>
+    <t>Smt. Malan Dilip Gholap</t>
+  </si>
+  <si>
+    <t>Keshavnagar Dist Latur</t>
+  </si>
+  <si>
+    <t>Mrs Vandna Sugriv Gaikwad</t>
+  </si>
+  <si>
+    <t>Advance Course  In Fashion Technology</t>
+  </si>
+  <si>
+    <t>Arvi Ta Latur Dist Latur</t>
+  </si>
+  <si>
+    <t>Smt. Jyoti Markade</t>
+  </si>
+  <si>
+    <t>Smt. Ayesha Pathan</t>
+  </si>
+  <si>
+    <t>Smt. Aruna Diggikar</t>
+  </si>
+  <si>
+    <t>Prakash Nagar Latur</t>
+  </si>
+  <si>
+    <t>Smt.Mina Kulkarni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial Year  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grant Received </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expenditure  on Training   </t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>NRC</t>
+  </si>
+  <si>
+    <t>2016-2017</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>3 Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details of Grants received for  Community Development Through Polytechnics (CDTP) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1197,6 +1323,32 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -1274,7 +1426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1322,6 +1474,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1331,6 +1486,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1343,6 +1510,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1354,6 +1530,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1925,23 +2119,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="2:9" s="7" customFormat="1" ht="45" customHeight="1">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="8" t="s">
         <v>28</v>
       </c>
@@ -1983,23 +2177,23 @@
       <c r="I5" s="9"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="2:9" ht="38.25">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
@@ -2041,23 +2235,23 @@
       <c r="I11" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="21"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="2:9" ht="38.25">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
@@ -2133,26 +2327,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="22"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="2:6" s="2" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" spans="2:6" s="2" customFormat="1" ht="12.75">
-      <c r="B4" s="20"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
@@ -2212,26 +2406,26 @@
       <c r="F9" s="10"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="22"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="2:6" ht="25.5" customHeight="1">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="20"/>
+      <c r="F13" s="25"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="20"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
@@ -2291,26 +2485,26 @@
       <c r="F19" s="10"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="27"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20" t="s">
+      <c r="D23" s="25"/>
+      <c r="E23" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="20"/>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="20"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
@@ -2370,26 +2564,26 @@
       <c r="F29" s="10"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="22"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20" t="s">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="20"/>
+      <c r="F33" s="25"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="20"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="8" t="s">
         <v>27</v>
       </c>
@@ -2476,10 +2670,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A23:H40"/>
+  <dimension ref="A3:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2487,340 +2681,952 @@
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="31.5703125" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="23" spans="1:8" ht="23.25" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="24" spans="1:8" ht="60" customHeight="1">
-      <c r="B24" s="4" t="s">
+    <row r="3" spans="2:8" ht="27" customHeight="1">
+      <c r="B3" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="2:8" ht="42" customHeight="1">
+      <c r="B4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D4" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B5" s="22">
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <v>2</v>
+      </c>
+      <c r="D5" s="22">
+        <v>3</v>
+      </c>
+      <c r="E5" s="22">
+        <v>4</v>
+      </c>
+      <c r="F5" s="22">
+        <v>5</v>
+      </c>
+      <c r="G5" s="22">
+        <v>6</v>
+      </c>
+      <c r="H5" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="30">
+      <c r="B6" s="22">
+        <v>1</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="22">
+        <v>12</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="22">
+        <v>13</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30">
+      <c r="B7" s="22">
+        <v>2</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="22">
+        <v>12</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="22">
+        <v>21</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="30">
+      <c r="B8" s="22">
+        <v>3</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="22">
+        <v>12</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="22">
+        <v>19</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30">
+      <c r="B9" s="22">
+        <v>4</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="22">
+        <v>12</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="22">
+        <v>22</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="42.75" customHeight="1">
+      <c r="B10" s="22">
+        <v>5</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="22">
+        <v>12</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="22">
+        <v>20</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B11" s="22">
+        <v>6</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="22">
+        <v>12</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="22">
+        <v>18</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="32.25" customHeight="1">
+      <c r="B12" s="22">
+        <v>7</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="22">
+        <v>12</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="22">
+        <v>21</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="25.5">
+      <c r="B13" s="22">
+        <v>8</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="22">
+        <v>12</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="22">
+        <v>21</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="30">
+      <c r="B14" s="22">
+        <v>9</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="22">
+        <v>12</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="22">
+        <v>16</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="45">
+      <c r="B15" s="22">
+        <v>10</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="22">
+        <v>12</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="22">
+        <v>22</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="30">
+      <c r="B16" s="22">
+        <v>11</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="22">
+        <v>4</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="22">
+        <v>15</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17" s="22">
+        <v>12</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="22">
+        <v>4</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="22">
+        <v>13</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="29.25" customHeight="1">
+      <c r="B18" s="22">
+        <v>13</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="22">
+        <v>12</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="22">
+        <v>21</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="29.25" customHeight="1">
+      <c r="B19" s="22">
+        <v>14</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="22">
+        <v>12</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="22">
+        <v>20</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30">
+      <c r="B20" s="22">
+        <v>15</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="22">
+        <v>12</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="22">
+        <v>20</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="29.25" customHeight="1">
+      <c r="B21" s="22">
+        <v>16</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="22">
+        <v>12</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="22">
+        <v>20</v>
+      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45">
+      <c r="B22" s="22">
+        <v>17</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="22">
+        <v>12</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="22">
+        <v>21</v>
+      </c>
+      <c r="G22" s="31"/>
+      <c r="H22" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="24.75" customHeight="1">
+      <c r="B23" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="C23" s="22">
+        <v>17</v>
+      </c>
+      <c r="D23" s="22">
+        <v>188</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22">
+        <v>323</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="26" spans="1:8" ht="23.25" customHeight="1">
+      <c r="A26" s="19"/>
+      <c r="B26" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+    </row>
+    <row r="27" spans="1:8" ht="60" customHeight="1">
+      <c r="B27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="G27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B25" s="4">
+    <row r="28" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B28" s="4">
         <v>1</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C28" s="4">
         <v>2</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D28" s="4">
         <v>3</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E28" s="4">
         <v>4</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F28" s="4">
         <v>5</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G28" s="4">
         <v>6</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H28" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="36" customHeight="1">
-      <c r="B26" s="17">
+    <row r="29" spans="1:8" ht="36" customHeight="1">
+      <c r="B29" s="18">
         <v>1</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="11">
-        <v>12</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="11">
-        <v>20</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="53.25" customHeight="1">
-      <c r="B27" s="17">
-        <v>2</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="11">
-        <v>12</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" s="11">
-        <v>20</v>
-      </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="48.75" customHeight="1">
-      <c r="B28" s="17">
-        <v>3</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="11">
-        <v>12</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="11">
-        <v>25</v>
-      </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="53.25" customHeight="1">
-      <c r="B29" s="17">
-        <v>4</v>
-      </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="18" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="11">
         <v>12</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F29" s="11">
         <v>20</v>
       </c>
-      <c r="G29" s="24"/>
+      <c r="G29" s="32" t="s">
+        <v>79</v>
+      </c>
       <c r="H29" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="35.25" customHeight="1">
-      <c r="B30" s="17">
-        <v>5</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="53.25" customHeight="1">
+      <c r="B30" s="18">
+        <v>2</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="D30" s="11">
         <v>12</v>
       </c>
       <c r="E30" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="11">
+        <v>20</v>
+      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="48.75" customHeight="1">
+      <c r="B31" s="18">
+        <v>3</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="11">
+        <v>12</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="11">
+        <v>25</v>
+      </c>
+      <c r="G31" s="32"/>
+      <c r="H31" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="53.25" customHeight="1">
+      <c r="B32" s="18">
+        <v>4</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="11">
+        <v>12</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F32" s="11">
+        <v>20</v>
+      </c>
+      <c r="G32" s="32"/>
+      <c r="H32" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="35.25" customHeight="1">
+      <c r="B33" s="18">
+        <v>5</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="11">
+        <v>12</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="11">
         <v>21</v>
       </c>
-      <c r="G30" s="24"/>
-      <c r="H30" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B31" s="4" t="s">
+      <c r="G33" s="32"/>
+      <c r="H33" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="25.5" customHeight="1">
+      <c r="B34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="11">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11">
+        <v>60</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11">
+        <v>106</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="36" spans="2:8" ht="20.25">
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="2:8" ht="24" customHeight="1">
+      <c r="B37" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="2:8" ht="65.25" customHeight="1">
+      <c r="B38" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="18" customHeight="1">
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4">
+        <v>2</v>
+      </c>
+      <c r="D39" s="4">
+        <v>3</v>
+      </c>
+      <c r="E39" s="4">
+        <v>4</v>
+      </c>
+      <c r="F39" s="4">
+        <v>5</v>
+      </c>
+      <c r="G39" s="4">
+        <v>6</v>
+      </c>
+      <c r="H39" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="36" customHeight="1">
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="14">
+        <v>12</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="14">
+        <v>20</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="53.25" customHeight="1">
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="11">
+        <v>12</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="11">
+        <v>21</v>
+      </c>
+      <c r="G41" s="34"/>
+      <c r="H41" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="26.25" customHeight="1">
+      <c r="B42" s="4">
+        <v>3</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="11">
+        <v>12</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="11">
+      <c r="F42" s="11">
+        <v>18</v>
+      </c>
+      <c r="G42" s="35"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="2:8" ht="29.25" customHeight="1">
+      <c r="B43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="11">
+        <v>3</v>
+      </c>
+      <c r="D43" s="11">
+        <v>36</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11">
+        <v>59</v>
+      </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="2:8" ht="29.25" customHeight="1">
+      <c r="B44" s="36"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="18">
+        <v>1</v>
+      </c>
+      <c r="C52" s="18">
+        <v>2</v>
+      </c>
+      <c r="D52" s="18">
+        <v>4</v>
+      </c>
+      <c r="E52" s="18">
         <v>5</v>
       </c>
-      <c r="D31" s="11">
-        <v>60</v>
-      </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11">
-        <v>106</v>
-      </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="33" spans="2:8" ht="20.25">
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="2:8" ht="24" customHeight="1">
-      <c r="B34" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-    </row>
-    <row r="35" spans="2:8" ht="65.25" customHeight="1">
-      <c r="B35" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="15" t="s">
+      <c r="F52" s="18">
+        <v>6</v>
+      </c>
+      <c r="G52" s="18">
+        <v>7</v>
+      </c>
+      <c r="H52" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="38">
+        <v>1</v>
+      </c>
+      <c r="C53" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F53" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="G53" s="40">
+        <v>158220</v>
+      </c>
+      <c r="H53" s="40">
+        <v>158220</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="38">
+        <v>2</v>
+      </c>
+      <c r="C54" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F54" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="G54" s="40">
+        <v>203753</v>
+      </c>
+      <c r="H54" s="40">
+        <v>203753</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="38">
+        <v>3</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F55" s="40">
+        <v>49500</v>
+      </c>
+      <c r="G55" s="40">
+        <v>269871</v>
+      </c>
+      <c r="H55" s="40">
+        <v>319371</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="18" customHeight="1">
-      <c r="B36" s="4">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4">
-        <v>2</v>
-      </c>
-      <c r="D36" s="4">
-        <v>3</v>
-      </c>
-      <c r="E36" s="4">
-        <v>4</v>
-      </c>
-      <c r="F36" s="4">
-        <v>5</v>
-      </c>
-      <c r="G36" s="4">
-        <v>6</v>
-      </c>
-      <c r="H36" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="36" customHeight="1">
-      <c r="B37" s="4">
-        <v>1</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="14">
-        <v>12</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="14">
-        <v>20</v>
-      </c>
-      <c r="G37" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="53.25" customHeight="1">
-      <c r="B38" s="4">
-        <v>2</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="11">
-        <v>12</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="11">
-        <v>21</v>
-      </c>
-      <c r="G38" s="26"/>
-      <c r="H38" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B39" s="4">
-        <v>3</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="11">
-        <v>12</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F39" s="11">
-        <v>18</v>
-      </c>
-      <c r="G39" s="27"/>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="2:8" ht="29.25" customHeight="1">
-      <c r="B40" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="11">
-        <v>3</v>
-      </c>
-      <c r="D40" s="11">
-        <v>36</v>
-      </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11">
-        <v>59</v>
-      </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="C56" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="40">
+        <v>49500</v>
+      </c>
+      <c r="G56" s="40">
+        <v>631844</v>
+      </c>
+      <c r="H56" s="40">
+        <v>681344</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="B34:H34"/>
+  <mergeCells count="11">
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="G6:G22"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="B37:H37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C9 9.4.1 Library facility table added
</commit_message>
<xml_diff>
--- a/Criterion 9/C9 Tables.xlsx
+++ b/Criterion 9/C9 Tables.xlsx
@@ -11,15 +11,16 @@
     <sheet name="9.1.1 availibilty of vision and" sheetId="2" r:id="rId2"/>
     <sheet name="9.2 Income at institute " sheetId="3" r:id="rId3"/>
     <sheet name="9.3 Department Specific budget" sheetId="4" r:id="rId4"/>
-    <sheet name="9.5 Community Development" sheetId="5" r:id="rId5"/>
-    <sheet name="9.6 Alumini Performance and con" sheetId="6" r:id="rId6"/>
+    <sheet name="9.4 Libarary and Internet" sheetId="7" r:id="rId5"/>
+    <sheet name="9.5 Community Development" sheetId="5" r:id="rId6"/>
+    <sheet name="9.6 Alumini Performance and con" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="154">
   <si>
     <t>CRITERION 9</t>
   </si>
@@ -1246,6 +1247,54 @@
   </si>
   <si>
     <t xml:space="preserve">Details of Grants received for  Community Development Through Polytechnics (CDTP) </t>
+  </si>
+  <si>
+    <t>Sr No</t>
+  </si>
+  <si>
+    <t>Used By</t>
+  </si>
+  <si>
+    <t>Area (Sq. M)</t>
+  </si>
+  <si>
+    <t>Available Furniture /  Facility</t>
+  </si>
+  <si>
+    <t>Utilization Purpose</t>
+  </si>
+  <si>
+    <t>Fans</t>
+  </si>
+  <si>
+    <t>Name of Facility</t>
+  </si>
+  <si>
+    <t>All Students Teaching and Non-teching staff</t>
+  </si>
+  <si>
+    <t>Notice Boards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internet </t>
+  </si>
+  <si>
+    <t>Yes/2 Nos</t>
+  </si>
+  <si>
+    <t>Book Cupboards</t>
+  </si>
+  <si>
+    <t>Tables/Desks/Sofas</t>
+  </si>
+  <si>
+    <t>No Of PCs</t>
+  </si>
+  <si>
+    <t>All library Facility is utilised by all Students, Teaching and non-teaching staff</t>
+  </si>
+  <si>
+    <t>Lanterns</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1498,6 +1547,18 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1508,6 +1569,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1531,23 +1598,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2119,23 +2177,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="2:9" s="7" customFormat="1" ht="45" customHeight="1">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
       <c r="I3" s="8" t="s">
         <v>28</v>
       </c>
@@ -2177,23 +2235,23 @@
       <c r="I5" s="9"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="38.25">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
@@ -2235,23 +2293,23 @@
       <c r="I11" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="26"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="2:9" ht="38.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25" t="s">
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
@@ -2327,26 +2385,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="2:6" s="2" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="25"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="2:6" s="2" customFormat="1" ht="12.75">
-      <c r="B4" s="25"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
@@ -2406,26 +2464,26 @@
       <c r="F9" s="10"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="27"/>
+      <c r="E12" s="31"/>
     </row>
     <row r="13" spans="2:6" ht="25.5" customHeight="1">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="29"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="25"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
@@ -2485,26 +2543,26 @@
       <c r="F19" s="10"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="27"/>
+      <c r="E22" s="31"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25" t="s">
+      <c r="D23" s="29"/>
+      <c r="E23" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="25"/>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="25"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
@@ -2564,26 +2622,26 @@
       <c r="F29" s="10"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="27"/>
+      <c r="E32" s="31"/>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25" t="s">
+      <c r="D33" s="29"/>
+      <c r="E33" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="25"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="8" t="s">
         <v>27</v>
       </c>
@@ -2670,9 +2728,124 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C4:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:14" ht="15" customHeight="1">
+      <c r="C4" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" ht="42.75" customHeight="1">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="N5" s="42"/>
+    </row>
+    <row r="6" spans="3:14" ht="87.75" customHeight="1">
+      <c r="C6" s="44">
+        <v>1</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B49" sqref="B49:H49"/>
     </sheetView>
   </sheetViews>
@@ -2689,15 +2862,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="27" customHeight="1">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="2:8" ht="42" customHeight="1">
       <c r="B4" s="4" t="s">
@@ -2761,7 +2934,7 @@
       <c r="F6" s="22">
         <v>13</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="35" t="s">
         <v>109</v>
       </c>
       <c r="H6" s="22" t="s">
@@ -2784,7 +2957,7 @@
       <c r="F7" s="22">
         <v>21</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="22" t="s">
         <v>112</v>
       </c>
@@ -2805,7 +2978,7 @@
       <c r="F8" s="22">
         <v>19</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="22" t="s">
         <v>99</v>
       </c>
@@ -2826,7 +2999,7 @@
       <c r="F9" s="22">
         <v>22</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="22" t="s">
         <v>76</v>
       </c>
@@ -2847,7 +3020,7 @@
       <c r="F10" s="22">
         <v>20</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="22" t="s">
         <v>76</v>
       </c>
@@ -2868,7 +3041,7 @@
       <c r="F11" s="22">
         <v>18</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="22" t="s">
         <v>96</v>
       </c>
@@ -2889,7 +3062,7 @@
       <c r="F12" s="22">
         <v>21</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="22" t="s">
         <v>112</v>
       </c>
@@ -2910,7 +3083,7 @@
       <c r="F13" s="22">
         <v>21</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="36"/>
       <c r="H13" s="22" t="s">
         <v>117</v>
       </c>
@@ -2931,7 +3104,7 @@
       <c r="F14" s="22">
         <v>16</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="22" t="s">
         <v>119</v>
       </c>
@@ -2952,7 +3125,7 @@
       <c r="F15" s="22">
         <v>22</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="22" t="s">
         <v>76</v>
       </c>
@@ -2973,7 +3146,7 @@
       <c r="F16" s="22">
         <v>15</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="36"/>
       <c r="H16" s="22" t="s">
         <v>76</v>
       </c>
@@ -2994,7 +3167,7 @@
       <c r="F17" s="22">
         <v>13</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="22" t="s">
         <v>112</v>
       </c>
@@ -3015,7 +3188,7 @@
       <c r="F18" s="22">
         <v>21</v>
       </c>
-      <c r="G18" s="30"/>
+      <c r="G18" s="36"/>
       <c r="H18" s="22" t="s">
         <v>122</v>
       </c>
@@ -3036,7 +3209,7 @@
       <c r="F19" s="22">
         <v>20</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="36"/>
       <c r="H19" s="22" t="s">
         <v>123</v>
       </c>
@@ -3057,7 +3230,7 @@
       <c r="F20" s="22">
         <v>20</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="22" t="s">
         <v>124</v>
       </c>
@@ -3078,7 +3251,7 @@
       <c r="F21" s="22">
         <v>20</v>
       </c>
-      <c r="G21" s="30"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="22" t="s">
         <v>126</v>
       </c>
@@ -3099,7 +3272,7 @@
       <c r="F22" s="22">
         <v>21</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="22" t="s">
         <v>76</v>
       </c>
@@ -3123,15 +3296,15 @@
     </row>
     <row r="26" spans="1:8" ht="23.25" customHeight="1">
       <c r="A26" s="19"/>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8" ht="60" customHeight="1">
       <c r="B27" s="4" t="s">
@@ -3195,7 +3368,7 @@
       <c r="F29" s="11">
         <v>20</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="38" t="s">
         <v>79</v>
       </c>
       <c r="H29" s="11" t="s">
@@ -3218,7 +3391,7 @@
       <c r="F30" s="11">
         <v>20</v>
       </c>
-      <c r="G30" s="32"/>
+      <c r="G30" s="38"/>
       <c r="H30" s="11" t="s">
         <v>93</v>
       </c>
@@ -3239,7 +3412,7 @@
       <c r="F31" s="11">
         <v>25</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="38"/>
       <c r="H31" s="11" t="s">
         <v>94</v>
       </c>
@@ -3260,7 +3433,7 @@
       <c r="F32" s="11">
         <v>20</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="38"/>
       <c r="H32" s="11" t="s">
         <v>95</v>
       </c>
@@ -3281,7 +3454,7 @@
       <c r="F33" s="11">
         <v>21</v>
       </c>
-      <c r="G33" s="32"/>
+      <c r="G33" s="38"/>
       <c r="H33" s="11" t="s">
         <v>96</v>
       </c>
@@ -3307,15 +3480,15 @@
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:8" ht="24" customHeight="1">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="2:8" ht="65.25" customHeight="1">
       <c r="B38" s="15" t="s">
@@ -3379,7 +3552,7 @@
       <c r="F40" s="14">
         <v>20</v>
       </c>
-      <c r="G40" s="33" t="s">
+      <c r="G40" s="39" t="s">
         <v>79</v>
       </c>
       <c r="H40" s="11" t="s">
@@ -3402,7 +3575,7 @@
       <c r="F41" s="11">
         <v>21</v>
       </c>
-      <c r="G41" s="34"/>
+      <c r="G41" s="40"/>
       <c r="H41" s="11" t="s">
         <v>76</v>
       </c>
@@ -3423,7 +3596,7 @@
       <c r="F42" s="11">
         <v>18</v>
       </c>
-      <c r="G42" s="35"/>
+      <c r="G42" s="41"/>
       <c r="H42" s="11"/>
     </row>
     <row r="43" spans="2:8" ht="29.25" customHeight="1">
@@ -3444,45 +3617,45 @@
       <c r="H43" s="11"/>
     </row>
     <row r="44" spans="2:8" ht="29.25" customHeight="1">
-      <c r="B44" s="36"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="39" t="s">
+      <c r="C50" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="39" t="s">
+      <c r="D50" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39" t="s">
+      <c r="E50" s="32"/>
+      <c r="F50" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
     </row>
     <row r="51" spans="2:8">
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="18" t="s">
         <v>130</v>
       </c>
@@ -3523,117 +3696,117 @@
       </c>
     </row>
     <row r="53" spans="2:8">
-      <c r="B53" s="38">
+      <c r="B53" s="27">
         <v>1</v>
       </c>
-      <c r="C53" s="38" t="s">
+      <c r="C53" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="38" t="s">
+      <c r="D53" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="E53" s="38" t="s">
+      <c r="E53" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="F53" s="38" t="s">
+      <c r="F53" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="G53" s="40">
+      <c r="G53" s="28">
         <v>158220</v>
       </c>
-      <c r="H53" s="40">
+      <c r="H53" s="28">
         <v>158220</v>
       </c>
     </row>
     <row r="54" spans="2:8">
-      <c r="B54" s="38">
+      <c r="B54" s="27">
         <v>2</v>
       </c>
-      <c r="C54" s="38" t="s">
+      <c r="C54" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="38" t="s">
+      <c r="D54" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="E54" s="38" t="s">
+      <c r="E54" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="F54" s="38" t="s">
+      <c r="F54" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="40">
+      <c r="G54" s="28">
         <v>203753</v>
       </c>
-      <c r="H54" s="40">
+      <c r="H54" s="28">
         <v>203753</v>
       </c>
     </row>
     <row r="55" spans="2:8">
-      <c r="B55" s="38">
+      <c r="B55" s="27">
         <v>3</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="C55" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="E55" s="38" t="s">
+      <c r="E55" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="F55" s="40">
+      <c r="F55" s="28">
         <v>49500</v>
       </c>
-      <c r="G55" s="40">
+      <c r="G55" s="28">
         <v>269871</v>
       </c>
-      <c r="H55" s="40">
+      <c r="H55" s="28">
         <v>319371</v>
       </c>
     </row>
     <row r="56" spans="2:8">
-      <c r="B56" s="38" t="s">
+      <c r="B56" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="38" t="s">
+      <c r="C56" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D56" s="38" t="s">
+      <c r="D56" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="E56" s="38" t="s">
+      <c r="E56" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="F56" s="40">
+      <c r="F56" s="28">
         <v>49500</v>
       </c>
-      <c r="G56" s="40">
+      <c r="G56" s="28">
         <v>631844</v>
       </c>
-      <c r="H56" s="40">
+      <c r="H56" s="28">
         <v>681344</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="B49:H49"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="G6:G22"/>
     <mergeCell ref="B26:H26"/>
     <mergeCell ref="G29:G33"/>
     <mergeCell ref="G40:G42"/>
     <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="B49:H49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
C9 Library and Internet tables added
</commit_message>
<xml_diff>
--- a/Criterion 9/C9 Tables.xlsx
+++ b/Criterion 9/C9 Tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="182">
   <si>
     <t>CRITERION 9</t>
   </si>
@@ -1295,6 +1295,90 @@
   </si>
   <si>
     <t>Lanterns</t>
+  </si>
+  <si>
+    <t>Facility in Libarary</t>
+  </si>
+  <si>
+    <t>Availability/Utilization</t>
+  </si>
+  <si>
+    <t>Book Bank facility</t>
+  </si>
+  <si>
+    <t>Reprography</t>
+  </si>
+  <si>
+    <t>Centralized Internet Lab</t>
+  </si>
+  <si>
+    <t>Reading Room Facility</t>
+  </si>
+  <si>
+    <t>Reference section</t>
+  </si>
+  <si>
+    <t>Online Searching Facility (OPAC)</t>
+  </si>
+  <si>
+    <t>Magazines and periodicals</t>
+  </si>
+  <si>
+    <t>News Papers</t>
+  </si>
+  <si>
+    <t>Internet Facility</t>
+  </si>
+  <si>
+    <t>Educational CDs/DVDs/Cassette</t>
+  </si>
+  <si>
+    <t>Library Management Software</t>
+  </si>
+  <si>
+    <t>Quantity/Nos</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Book/Title Scheme</t>
+  </si>
+  <si>
+    <t>Development of library</t>
+  </si>
+  <si>
+    <t>Social welfare book bank</t>
+  </si>
+  <si>
+    <t>Book bank</t>
+  </si>
+  <si>
+    <t>Any Other Scheme-</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Cost in Rs.</t>
+  </si>
+  <si>
+    <t>No. of Books</t>
+  </si>
+  <si>
+    <t>Titles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Volumes</t>
+  </si>
+  <si>
+    <t>National journals</t>
+  </si>
+  <si>
+    <t>International journals</t>
+  </si>
+  <si>
+    <t>DELNET Facility</t>
   </si>
 </sst>
 </file>
@@ -1475,7 +1559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1547,6 +1631,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1598,13 +1685,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1934,7 +2025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2162,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2177,23 +2268,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="30"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="2:9" s="7" customFormat="1" ht="45" customHeight="1">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
       <c r="I3" s="8" t="s">
         <v>28</v>
       </c>
@@ -2235,23 +2326,23 @@
       <c r="I5" s="9"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="2:9" ht="38.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
@@ -2293,23 +2384,23 @@
       <c r="I11" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="2:9" ht="38.25">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
@@ -2371,7 +2462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
@@ -2385,26 +2476,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="31"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="2:6" s="2" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="2:6" s="2" customFormat="1" ht="12.75">
-      <c r="B4" s="29"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
@@ -2464,26 +2555,26 @@
       <c r="F9" s="10"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" spans="2:6" ht="25.5" customHeight="1">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="30"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="29"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
@@ -2543,26 +2634,26 @@
       <c r="F19" s="10"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29" t="s">
+      <c r="D23" s="30"/>
+      <c r="E23" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="29"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="29"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
@@ -2622,26 +2713,26 @@
       <c r="F29" s="10"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="31"/>
+      <c r="E32" s="32"/>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29" t="s">
+      <c r="D33" s="30"/>
+      <c r="E33" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="29"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="29"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="8" t="s">
         <v>27</v>
       </c>
@@ -2728,104 +2819,423 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:N6"/>
+  <dimension ref="C3:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="45"/>
+    <col min="4" max="4" width="34.85546875" style="45" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="45" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="45" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="45"/>
+    <col min="10" max="10" width="8.28515625" style="45" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="45" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="45" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="45" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="45" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
+    <row r="3" spans="3:14">
+      <c r="J3" s="2"/>
+    </row>
     <row r="4" spans="3:14" ht="15" customHeight="1">
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="42" t="s">
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="46" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="3:14" ht="42.75" customHeight="1">
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="24" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="N5" s="42"/>
+      <c r="N5" s="46"/>
     </row>
     <row r="6" spans="3:14" ht="87.75" customHeight="1">
-      <c r="C6" s="44">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44" t="s">
+      <c r="L6" s="10"/>
+      <c r="M6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="25" t="s">
         <v>152</v>
       </c>
+    </row>
+    <row r="10" spans="3:14" ht="26.25" customHeight="1">
+      <c r="C10" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" ht="22.5" customHeight="1">
+      <c r="C11" s="10">
+        <v>1</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="3:14" ht="20.25" customHeight="1">
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="3:14" ht="20.25" customHeight="1">
+      <c r="C13" s="10">
+        <v>3</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="3:14" ht="20.25" customHeight="1">
+      <c r="C14" s="10">
+        <v>4</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="3:14" ht="20.25" customHeight="1">
+      <c r="C15" s="10">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="3:14" ht="20.25" customHeight="1">
+      <c r="C16" s="10">
+        <v>6</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C17" s="10">
+        <v>7</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C18" s="10">
+        <v>8</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C19" s="10">
+        <v>9</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C20" s="10">
+        <v>10</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C21" s="10">
+        <v>11</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C22" s="10">
+        <v>12</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C23" s="10">
+        <v>13</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C24" s="10">
+        <v>14</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C25" s="10">
+        <v>15</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C26" s="10">
+        <v>16</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C27" s="10">
+        <v>17</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C28" s="10">
+        <v>18</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C29" s="10">
+        <v>19</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="3:11" ht="20.25" customHeight="1">
+      <c r="C30" s="10">
+        <v>20</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="32" spans="3:11">
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="3:6" ht="20.25" customHeight="1">
+      <c r="C33" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="20.25" customHeight="1">
+      <c r="C34" s="10">
+        <v>1</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="3:6" ht="20.25" customHeight="1">
+      <c r="C35" s="10">
+        <v>2</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="3:6" ht="20.25" customHeight="1">
+      <c r="C36" s="10">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="3:6" ht="20.25" customHeight="1">
+      <c r="C37" s="10">
+        <v>4</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="3:6" ht="18" customHeight="1">
+      <c r="C38" s="10">
+        <v>5</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="3:6" ht="18" customHeight="1">
+      <c r="C39" s="10">
+        <v>6</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="3:6" ht="18" customHeight="1">
+      <c r="C40" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2845,7 +3255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H56"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B49" sqref="B49:H49"/>
     </sheetView>
   </sheetViews>
@@ -2862,15 +3272,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="27" customHeight="1">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="2:8" ht="42" customHeight="1">
       <c r="B4" s="4" t="s">
@@ -2934,7 +3344,7 @@
       <c r="F6" s="22">
         <v>13</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="36" t="s">
         <v>109</v>
       </c>
       <c r="H6" s="22" t="s">
@@ -2957,7 +3367,7 @@
       <c r="F7" s="22">
         <v>21</v>
       </c>
-      <c r="G7" s="36"/>
+      <c r="G7" s="37"/>
       <c r="H7" s="22" t="s">
         <v>112</v>
       </c>
@@ -2978,7 +3388,7 @@
       <c r="F8" s="22">
         <v>19</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="22" t="s">
         <v>99</v>
       </c>
@@ -2999,7 +3409,7 @@
       <c r="F9" s="22">
         <v>22</v>
       </c>
-      <c r="G9" s="36"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="22" t="s">
         <v>76</v>
       </c>
@@ -3020,7 +3430,7 @@
       <c r="F10" s="22">
         <v>20</v>
       </c>
-      <c r="G10" s="36"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="22" t="s">
         <v>76</v>
       </c>
@@ -3041,7 +3451,7 @@
       <c r="F11" s="22">
         <v>18</v>
       </c>
-      <c r="G11" s="36"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="22" t="s">
         <v>96</v>
       </c>
@@ -3062,7 +3472,7 @@
       <c r="F12" s="22">
         <v>21</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="22" t="s">
         <v>112</v>
       </c>
@@ -3083,7 +3493,7 @@
       <c r="F13" s="22">
         <v>21</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="22" t="s">
         <v>117</v>
       </c>
@@ -3104,7 +3514,7 @@
       <c r="F14" s="22">
         <v>16</v>
       </c>
-      <c r="G14" s="36"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="22" t="s">
         <v>119</v>
       </c>
@@ -3125,7 +3535,7 @@
       <c r="F15" s="22">
         <v>22</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="22" t="s">
         <v>76</v>
       </c>
@@ -3146,7 +3556,7 @@
       <c r="F16" s="22">
         <v>15</v>
       </c>
-      <c r="G16" s="36"/>
+      <c r="G16" s="37"/>
       <c r="H16" s="22" t="s">
         <v>76</v>
       </c>
@@ -3167,7 +3577,7 @@
       <c r="F17" s="22">
         <v>13</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="22" t="s">
         <v>112</v>
       </c>
@@ -3188,7 +3598,7 @@
       <c r="F18" s="22">
         <v>21</v>
       </c>
-      <c r="G18" s="36"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="22" t="s">
         <v>122</v>
       </c>
@@ -3209,7 +3619,7 @@
       <c r="F19" s="22">
         <v>20</v>
       </c>
-      <c r="G19" s="36"/>
+      <c r="G19" s="37"/>
       <c r="H19" s="22" t="s">
         <v>123</v>
       </c>
@@ -3230,7 +3640,7 @@
       <c r="F20" s="22">
         <v>20</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="37"/>
       <c r="H20" s="22" t="s">
         <v>124</v>
       </c>
@@ -3251,7 +3661,7 @@
       <c r="F21" s="22">
         <v>20</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="37"/>
       <c r="H21" s="22" t="s">
         <v>126</v>
       </c>
@@ -3272,7 +3682,7 @@
       <c r="F22" s="22">
         <v>21</v>
       </c>
-      <c r="G22" s="37"/>
+      <c r="G22" s="38"/>
       <c r="H22" s="22" t="s">
         <v>76</v>
       </c>
@@ -3296,15 +3706,15 @@
     </row>
     <row r="26" spans="1:8" ht="23.25" customHeight="1">
       <c r="A26" s="19"/>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" ht="60" customHeight="1">
       <c r="B27" s="4" t="s">
@@ -3368,7 +3778,7 @@
       <c r="F29" s="11">
         <v>20</v>
       </c>
-      <c r="G29" s="38" t="s">
+      <c r="G29" s="39" t="s">
         <v>79</v>
       </c>
       <c r="H29" s="11" t="s">
@@ -3391,7 +3801,7 @@
       <c r="F30" s="11">
         <v>20</v>
       </c>
-      <c r="G30" s="38"/>
+      <c r="G30" s="39"/>
       <c r="H30" s="11" t="s">
         <v>93</v>
       </c>
@@ -3412,7 +3822,7 @@
       <c r="F31" s="11">
         <v>25</v>
       </c>
-      <c r="G31" s="38"/>
+      <c r="G31" s="39"/>
       <c r="H31" s="11" t="s">
         <v>94</v>
       </c>
@@ -3433,7 +3843,7 @@
       <c r="F32" s="11">
         <v>20</v>
       </c>
-      <c r="G32" s="38"/>
+      <c r="G32" s="39"/>
       <c r="H32" s="11" t="s">
         <v>95</v>
       </c>
@@ -3454,7 +3864,7 @@
       <c r="F33" s="11">
         <v>21</v>
       </c>
-      <c r="G33" s="38"/>
+      <c r="G33" s="39"/>
       <c r="H33" s="11" t="s">
         <v>96</v>
       </c>
@@ -3480,15 +3890,15 @@
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:8" ht="24" customHeight="1">
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
     </row>
     <row r="38" spans="2:8" ht="65.25" customHeight="1">
       <c r="B38" s="15" t="s">
@@ -3552,7 +3962,7 @@
       <c r="F40" s="14">
         <v>20</v>
       </c>
-      <c r="G40" s="39" t="s">
+      <c r="G40" s="40" t="s">
         <v>79</v>
       </c>
       <c r="H40" s="11" t="s">
@@ -3575,7 +3985,7 @@
       <c r="F41" s="11">
         <v>21</v>
       </c>
-      <c r="G41" s="40"/>
+      <c r="G41" s="41"/>
       <c r="H41" s="11" t="s">
         <v>76</v>
       </c>
@@ -3596,7 +4006,7 @@
       <c r="F42" s="11">
         <v>18</v>
       </c>
-      <c r="G42" s="41"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="11"/>
     </row>
     <row r="43" spans="2:8" ht="29.25" customHeight="1">
@@ -3617,45 +4027,45 @@
       <c r="H43" s="11"/>
     </row>
     <row r="44" spans="2:8" ht="29.25" customHeight="1">
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="33" t="s">
+      <c r="B49" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="32" t="s">
+      <c r="B50" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="32" t="s">
+      <c r="D50" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32" t="s">
+      <c r="E50" s="33"/>
+      <c r="F50" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
     </row>
     <row r="51" spans="2:8">
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
       <c r="D51" s="18" t="s">
         <v>130</v>
       </c>
@@ -3696,94 +4106,94 @@
       </c>
     </row>
     <row r="53" spans="2:8">
-      <c r="B53" s="27">
+      <c r="B53" s="28">
         <v>1</v>
       </c>
-      <c r="C53" s="27" t="s">
+      <c r="C53" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="27" t="s">
+      <c r="D53" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="E53" s="27" t="s">
+      <c r="E53" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="F53" s="27" t="s">
+      <c r="F53" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="G53" s="28">
+      <c r="G53" s="29">
         <v>158220</v>
       </c>
-      <c r="H53" s="28">
+      <c r="H53" s="29">
         <v>158220</v>
       </c>
     </row>
     <row r="54" spans="2:8">
-      <c r="B54" s="27">
+      <c r="B54" s="28">
         <v>2</v>
       </c>
-      <c r="C54" s="27" t="s">
+      <c r="C54" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="27" t="s">
+      <c r="D54" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="E54" s="27" t="s">
+      <c r="E54" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="F54" s="27" t="s">
+      <c r="F54" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="28">
+      <c r="G54" s="29">
         <v>203753</v>
       </c>
-      <c r="H54" s="28">
+      <c r="H54" s="29">
         <v>203753</v>
       </c>
     </row>
     <row r="55" spans="2:8">
-      <c r="B55" s="27">
+      <c r="B55" s="28">
         <v>3</v>
       </c>
-      <c r="C55" s="27" t="s">
+      <c r="C55" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="27" t="s">
+      <c r="D55" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="E55" s="27" t="s">
+      <c r="E55" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="F55" s="28">
+      <c r="F55" s="29">
         <v>49500</v>
       </c>
-      <c r="G55" s="28">
+      <c r="G55" s="29">
         <v>269871</v>
       </c>
-      <c r="H55" s="28">
+      <c r="H55" s="29">
         <v>319371</v>
       </c>
     </row>
     <row r="56" spans="2:8">
-      <c r="B56" s="27" t="s">
+      <c r="B56" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D56" s="27" t="s">
+      <c r="D56" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="E56" s="27" t="s">
+      <c r="E56" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="F56" s="28">
+      <c r="F56" s="29">
         <v>49500</v>
       </c>
-      <c r="G56" s="28">
+      <c r="G56" s="29">
         <v>631844</v>
       </c>
-      <c r="H56" s="28">
+      <c r="H56" s="29">
         <v>681344</v>
       </c>
     </row>

</xml_diff>